<commit_message>
updates to worksheet - needs more work
</commit_message>
<xml_diff>
--- a/analyses/data/Exp.Individs.xlsx
+++ b/analyses/data/Exp.Individs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/freezingexperiment/analyses/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22800" windowHeight="13520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="8180" yWindow="1780" windowWidth="29940" windowHeight="21380" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
@@ -17,18 +22,18 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="256">
   <si>
     <t>Species</t>
   </si>
@@ -787,6 +792,15 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Potted?</t>
+  </si>
+  <si>
+    <t>Soil Moisture</t>
+  </si>
+  <si>
+    <t>Phenophase</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1266,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1266,14 +1280,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>231</v>
       </c>
@@ -1281,7 +1295,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>232</v>
       </c>
@@ -1289,7 +1303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>235</v>
       </c>
@@ -1303,7 +1317,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>236</v>
       </c>
@@ -1317,7 +1331,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>239</v>
       </c>
@@ -1331,27 +1345,27 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>242</v>
       </c>
@@ -1359,7 +1373,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>244</v>
       </c>
@@ -1367,7 +1381,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>246</v>
       </c>
@@ -1377,11 +1391,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1396,9 +1405,9 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1439,7 +1448,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1509,7 +1518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1547,7 +1556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1690,7 +1699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1719,7 +1728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1748,7 +1757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1806,7 +1815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1861,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1890,7 +1899,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1919,7 +1928,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1948,7 +1957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1974,7 +1983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2003,7 +2012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2032,7 +2041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -2057,7 +2066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2068,7 +2077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2082,7 +2091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2096,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2110,7 +2119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2121,7 +2130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2135,7 +2144,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2149,7 +2158,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2163,7 +2172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2188,26 +2197,24 @@
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I148"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:I1048576"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
@@ -2219,7 +2226,7 @@
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2247,8 +2254,17 @@
       <c r="I1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>253</v>
+      </c>
+      <c r="K1" t="s">
+        <v>254</v>
+      </c>
+      <c r="L1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2277,7 +2293,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2306,7 +2322,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -2335,7 +2351,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2364,7 +2380,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2393,7 +2409,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2422,7 +2438,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2451,7 +2467,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -2480,7 +2496,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -2509,7 +2525,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2538,7 +2554,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2567,7 +2583,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -2596,7 +2612,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2625,7 +2641,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2654,7 +2670,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2683,7 +2699,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2712,7 +2728,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2741,7 +2757,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2770,7 +2786,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -2799,7 +2815,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2828,7 +2844,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2857,7 +2873,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2886,7 +2902,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2915,7 +2931,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2944,7 +2960,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2973,7 +2989,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -3002,7 +3018,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -3031,7 +3047,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -3060,7 +3076,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -3089,7 +3105,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3118,7 +3134,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3147,7 +3163,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -3176,7 +3192,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -3205,7 +3221,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -3234,7 +3250,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -3263,7 +3279,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -3292,7 +3308,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -3321,7 +3337,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -3350,7 +3366,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -3379,7 +3395,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -3408,7 +3424,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -3437,7 +3453,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -3466,7 +3482,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -3495,7 +3511,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -3524,7 +3540,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>37</v>
       </c>
@@ -3553,7 +3569,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -3582,7 +3598,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -3611,7 +3627,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -3640,7 +3656,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -3669,7 +3685,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -3698,7 +3714,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>40</v>
       </c>
@@ -3727,7 +3743,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -3756,7 +3772,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -3785,7 +3801,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -3814,7 +3830,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -3843,7 +3859,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -3872,7 +3888,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -3901,7 +3917,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>73</v>
       </c>
@@ -3930,7 +3946,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -3959,7 +3975,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3988,7 +4004,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -4017,7 +4033,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -4046,7 +4062,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>74</v>
       </c>
@@ -4075,7 +4091,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>75</v>
       </c>
@@ -4104,7 +4120,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -4133,7 +4149,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -4162,7 +4178,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -4191,7 +4207,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -4220,7 +4236,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -4249,7 +4265,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>46</v>
       </c>
@@ -4278,7 +4294,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>46</v>
       </c>
@@ -4307,7 +4323,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>46</v>
       </c>
@@ -4336,7 +4352,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -4365,7 +4381,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>47</v>
       </c>
@@ -4394,7 +4410,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>47</v>
       </c>
@@ -4423,7 +4439,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>71</v>
       </c>
@@ -4452,7 +4468,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>45</v>
       </c>
@@ -4481,7 +4497,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>45</v>
       </c>
@@ -4510,7 +4526,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>45</v>
       </c>
@@ -4539,7 +4555,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>66</v>
       </c>
@@ -4568,7 +4584,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>66</v>
       </c>
@@ -4597,7 +4613,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>66</v>
       </c>
@@ -4626,7 +4642,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>66</v>
       </c>
@@ -4655,7 +4671,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>66</v>
       </c>
@@ -4684,7 +4700,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>66</v>
       </c>
@@ -4713,7 +4729,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>66</v>
       </c>
@@ -4742,7 +4758,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>66</v>
       </c>
@@ -4771,7 +4787,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>66</v>
       </c>
@@ -4800,7 +4816,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>66</v>
       </c>
@@ -4829,7 +4845,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>72</v>
       </c>
@@ -4858,7 +4874,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>68</v>
       </c>
@@ -4887,7 +4903,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>68</v>
       </c>
@@ -4916,7 +4932,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>68</v>
       </c>
@@ -4945,7 +4961,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -4974,7 +4990,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>57</v>
       </c>
@@ -5003,7 +5019,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>57</v>
       </c>
@@ -5032,7 +5048,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>64</v>
       </c>
@@ -5061,7 +5077,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>70</v>
       </c>
@@ -5090,7 +5106,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>67</v>
       </c>
@@ -5119,7 +5135,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>65</v>
       </c>
@@ -5148,7 +5164,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>65</v>
       </c>
@@ -5177,7 +5193,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>62</v>
       </c>
@@ -5206,7 +5222,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>62</v>
       </c>
@@ -5235,7 +5251,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>62</v>
       </c>
@@ -5264,7 +5280,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>62</v>
       </c>
@@ -5293,7 +5309,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>62</v>
       </c>
@@ -5322,7 +5338,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>62</v>
       </c>
@@ -5351,7 +5367,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>62</v>
       </c>
@@ -5380,7 +5396,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>61</v>
       </c>
@@ -5409,7 +5425,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>63</v>
       </c>
@@ -5438,7 +5454,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>63</v>
       </c>
@@ -5467,7 +5483,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>49</v>
       </c>
@@ -5496,7 +5512,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>49</v>
       </c>
@@ -5525,7 +5541,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>49</v>
       </c>
@@ -5554,7 +5570,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>49</v>
       </c>
@@ -5583,7 +5599,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>49</v>
       </c>
@@ -5612,7 +5628,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>49</v>
       </c>
@@ -5641,7 +5657,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>49</v>
       </c>
@@ -5670,7 +5686,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>49</v>
       </c>
@@ -5699,7 +5715,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>53</v>
       </c>
@@ -5728,7 +5744,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>53</v>
       </c>
@@ -5757,7 +5773,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>53</v>
       </c>
@@ -5786,7 +5802,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>53</v>
       </c>
@@ -5815,7 +5831,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>53</v>
       </c>
@@ -5844,7 +5860,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>50</v>
       </c>
@@ -5873,7 +5889,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>50</v>
       </c>
@@ -5902,7 +5918,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>52</v>
       </c>
@@ -5931,7 +5947,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>52</v>
       </c>
@@ -5960,7 +5976,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>52</v>
       </c>
@@ -5989,7 +6005,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>52</v>
       </c>
@@ -6018,7 +6034,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>52</v>
       </c>
@@ -6047,7 +6063,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>54</v>
       </c>
@@ -6076,7 +6092,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>54</v>
       </c>
@@ -6105,7 +6121,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>54</v>
       </c>
@@ -6134,7 +6150,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>54</v>
       </c>
@@ -6163,7 +6179,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>54</v>
       </c>
@@ -6192,7 +6208,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>55</v>
       </c>
@@ -6221,7 +6237,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>55</v>
       </c>
@@ -6250,7 +6266,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>81</v>
       </c>
@@ -6279,7 +6295,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>81</v>
       </c>
@@ -6308,7 +6324,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>51</v>
       </c>
@@ -6337,7 +6353,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>51</v>
       </c>
@@ -6366,7 +6382,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>51</v>
       </c>
@@ -6395,7 +6411,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>51</v>
       </c>
@@ -6424,7 +6440,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>51</v>
       </c>
@@ -6453,7 +6469,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>56</v>
       </c>
@@ -6482,7 +6498,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>56</v>
       </c>
@@ -6513,12 +6529,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup scale="80" fitToHeight="4" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
</xml_diff>